<commit_message>
soli test correction #2
Former-commit-id: c035b72e206ee57137b997269abb1f06f9156856
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_soli.xlsx
+++ b/tests/test_data/test_dfs_soli.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>tu_id</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>child</t>
+  </si>
+  <si>
+    <t>incometax_tu</t>
   </si>
 </sst>
 </file>
@@ -407,20 +410,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W24"/>
+  <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="12" max="13" width="13.7109375" customWidth="1"/>
-    <col min="14" max="14" width="16.7109375" customWidth="1"/>
-    <col min="23" max="23" width="9.140625" style="1"/>
+    <col min="13" max="14" width="13.7109375" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -437,29 +440,32 @@
         <v>11</v>
       </c>
       <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="3" t="s">
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>6</v>
       </c>
-      <c r="W1"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>B2</f>
         <v>1</v>
@@ -477,32 +483,36 @@
         <v>0</v>
       </c>
       <c r="F2">
+        <f>MIN(G2,H2)</f>
         <v>5000</v>
       </c>
       <c r="G2">
+        <v>5000</v>
+      </c>
+      <c r="H2">
         <v>6000</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>150</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>2016</v>
       </c>
-      <c r="L2" s="4">
-        <f>M2/2</f>
+      <c r="M2" s="4">
+        <f>N2/2</f>
         <v>141.625</v>
       </c>
-      <c r="M2" s="4">
-        <f>MIN(0.055*O2,MAX(0.2*O2,972))</f>
+      <c r="N2" s="4">
+        <f>MIN(0.055*P2,MAX(0.2*P2,972))</f>
         <v>283.25</v>
       </c>
-      <c r="O2">
-        <f>F2+H2</f>
+      <c r="P2">
+        <f>G2+I2</f>
         <v>5150</v>
       </c>
-      <c r="W2"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X2"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -519,32 +529,36 @@
         <v>0</v>
       </c>
       <c r="F3">
+        <f t="shared" ref="F3:F7" si="0">MIN(G3,H3)</f>
         <v>5000</v>
       </c>
       <c r="G3">
+        <v>5000</v>
+      </c>
+      <c r="H3">
         <v>6000</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>150</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>2016</v>
       </c>
-      <c r="L3" s="4">
-        <f>M3/2</f>
+      <c r="M3" s="4">
+        <f>N3/2</f>
         <v>141.625</v>
       </c>
-      <c r="M3" s="4">
-        <f>MIN(0.055*O3,MAX(0.2*O3,972))</f>
+      <c r="N3" s="4">
+        <f>MIN(0.055*P3,MAX(0.2*P3,972))</f>
         <v>283.25</v>
       </c>
-      <c r="O3">
-        <f t="shared" ref="O3:O7" si="0">F3+H3</f>
+      <c r="P3">
+        <f t="shared" ref="P3:P7" si="1">G3+I3</f>
         <v>5150</v>
       </c>
-      <c r="W3"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X3"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -561,6 +575,7 @@
         <v>1</v>
       </c>
       <c r="F4">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
@@ -569,22 +584,25 @@
       <c r="H4">
         <v>0</v>
       </c>
-      <c r="J4">
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="K4">
         <v>2016</v>
       </c>
-      <c r="L4" s="4">
-        <v>0</v>
-      </c>
       <c r="M4" s="4">
         <v>0</v>
       </c>
-      <c r="O4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W4"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="N4" s="4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X4"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -601,34 +619,38 @@
         <v>0</v>
       </c>
       <c r="F5">
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="G5">
+        <v>20000</v>
+      </c>
+      <c r="H5">
         <v>21000</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>50</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>2012</v>
       </c>
-      <c r="L5" s="4">
-        <f>M5</f>
+      <c r="M5" s="4">
+        <f>N5</f>
         <v>1102.75</v>
       </c>
-      <c r="M5" s="4">
-        <f>MIN(0.055*O5,MAX(0.2*O5,972))</f>
+      <c r="N5" s="4">
+        <f>MIN(0.055*P5,MAX(0.2*P5,972))</f>
         <v>1102.75</v>
       </c>
-      <c r="O5">
-        <f t="shared" si="0"/>
+      <c r="P5">
+        <f t="shared" si="1"/>
         <v>20050</v>
       </c>
-      <c r="W5"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X5"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" ref="A6:A7" si="1">B6</f>
+        <f t="shared" ref="A6:A7" si="2">B6</f>
         <v>4</v>
       </c>
       <c r="B6">
@@ -644,34 +666,38 @@
         <v>0</v>
       </c>
       <c r="F6">
+        <f t="shared" si="0"/>
         <v>50000</v>
       </c>
       <c r="G6">
+        <v>50000</v>
+      </c>
+      <c r="H6">
         <v>55000</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="J6">
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="K6">
         <v>2003</v>
       </c>
-      <c r="L6" s="4">
-        <f t="shared" ref="L6:L7" si="2">M6</f>
+      <c r="M6" s="4">
+        <f t="shared" ref="M6:M7" si="3">N6</f>
         <v>3025</v>
       </c>
-      <c r="M6" s="4">
-        <f>MIN(0.055*O6,MAX(0.2*O6,972))</f>
+      <c r="N6" s="4">
+        <f>MIN(0.055*P6,MAX(0.2*P6,972))</f>
         <v>3025</v>
       </c>
-      <c r="O6">
-        <f>G6</f>
+      <c r="P6">
+        <f>H6</f>
         <v>55000</v>
       </c>
-      <c r="W6"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X6"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="B7">
@@ -687,83 +713,87 @@
         <v>0</v>
       </c>
       <c r="F7">
+        <f t="shared" si="0"/>
         <v>200000</v>
       </c>
       <c r="G7">
         <v>200000</v>
       </c>
       <c r="H7">
+        <v>200000</v>
+      </c>
+      <c r="I7">
         <v>50</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>2018</v>
       </c>
-      <c r="L7" s="4">
-        <f t="shared" si="2"/>
+      <c r="M7" s="4">
+        <f t="shared" si="3"/>
         <v>11002.75</v>
       </c>
-      <c r="M7" s="4">
-        <f>MIN(0.055*O7,MAX(0.2*O7,972))</f>
+      <c r="N7" s="4">
+        <f>MIN(0.055*P7,MAX(0.2*P7,972))</f>
         <v>11002.75</v>
       </c>
-      <c r="O7">
-        <f t="shared" si="0"/>
+      <c r="P7">
+        <f t="shared" si="1"/>
         <v>200050</v>
       </c>
-      <c r="W7"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L8" s="4"/>
+      <c r="X7"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M8" s="4"/>
-      <c r="W8" s="2"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="W9" s="2"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="W10" s="2"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="W11" s="2"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="W12" s="2"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="W13" s="2"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="W14" s="2"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="W15" s="2"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="W16" s="2"/>
-    </row>
-    <row r="17" spans="23:23" x14ac:dyDescent="0.25">
-      <c r="W17" s="2"/>
-    </row>
-    <row r="18" spans="23:23" x14ac:dyDescent="0.25">
-      <c r="W18" s="2"/>
-    </row>
-    <row r="19" spans="23:23" x14ac:dyDescent="0.25">
-      <c r="W19" s="2"/>
-    </row>
-    <row r="20" spans="23:23" x14ac:dyDescent="0.25">
-      <c r="W20" s="2"/>
-    </row>
-    <row r="21" spans="23:23" x14ac:dyDescent="0.25">
-      <c r="W21" s="2"/>
-    </row>
-    <row r="22" spans="23:23" x14ac:dyDescent="0.25">
-      <c r="W22" s="2"/>
-    </row>
-    <row r="23" spans="23:23" x14ac:dyDescent="0.25">
-      <c r="W23" s="2"/>
-    </row>
-    <row r="24" spans="23:23" x14ac:dyDescent="0.25">
-      <c r="W24" s="2"/>
+      <c r="N8" s="4"/>
+      <c r="X8" s="2"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X9" s="2"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X10" s="2"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X11" s="2"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X12" s="2"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X13" s="2"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X14" s="2"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X15" s="2"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X16" s="2"/>
+    </row>
+    <row r="17" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X17" s="2"/>
+    </row>
+    <row r="18" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X18" s="2"/>
+    </row>
+    <row r="19" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X19" s="2"/>
+    </row>
+    <row r="20" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X20" s="2"/>
+    </row>
+    <row r="21" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X21" s="2"/>
+    </row>
+    <row r="22" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X22" s="2"/>
+    </row>
+    <row r="23" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X23" s="2"/>
+    </row>
+    <row r="24" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X24" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
soli Bug was solved the wrong way (output should be in monthly terms), soli test adjusted accordingly
Former-commit-id: 3df225d1074d7aa375534faaa50abe4dfcda7c9c
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_soli.xlsx
+++ b/tests/test_data/test_dfs_soli.xlsx
@@ -413,7 +413,7 @@
   <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,11 +500,11 @@
       </c>
       <c r="M2" s="4">
         <f>N2/2</f>
-        <v>141.625</v>
+        <v>11.802083333333334</v>
       </c>
       <c r="N2" s="4">
-        <f>MIN(0.055*P2,MAX(0.2*P2,972))</f>
-        <v>283.25</v>
+        <f>MIN(0.055*P2,MAX(0.2*P2,972))/12</f>
+        <v>23.604166666666668</v>
       </c>
       <c r="P2">
         <f>G2+I2</f>
@@ -546,11 +546,11 @@
       </c>
       <c r="M3" s="4">
         <f>N3/2</f>
-        <v>141.625</v>
+        <v>11.802083333333334</v>
       </c>
       <c r="N3" s="4">
-        <f>MIN(0.055*P3,MAX(0.2*P3,972))</f>
-        <v>283.25</v>
+        <f>MIN(0.055*P3,MAX(0.2*P3,972))/12</f>
+        <v>23.604166666666668</v>
       </c>
       <c r="P3">
         <f t="shared" ref="P3:P7" si="1">G3+I3</f>
@@ -636,11 +636,11 @@
       </c>
       <c r="M5" s="4">
         <f>N5</f>
-        <v>1102.75</v>
+        <v>91.895833333333329</v>
       </c>
       <c r="N5" s="4">
-        <f>MIN(0.055*P5,MAX(0.2*P5,972))</f>
-        <v>1102.75</v>
+        <f>MIN(0.055*P5,MAX(0.2*P5,972))/12</f>
+        <v>91.895833333333329</v>
       </c>
       <c r="P5">
         <f t="shared" si="1"/>
@@ -683,11 +683,11 @@
       </c>
       <c r="M6" s="4">
         <f t="shared" ref="M6:M7" si="3">N6</f>
-        <v>3025</v>
+        <v>252.08333333333334</v>
       </c>
       <c r="N6" s="4">
-        <f>MIN(0.055*P6,MAX(0.2*P6,972))</f>
-        <v>3025</v>
+        <f>MIN(0.055*P6,MAX(0.2*P6,972))/12</f>
+        <v>252.08333333333334</v>
       </c>
       <c r="P6">
         <f>H6</f>
@@ -730,11 +730,11 @@
       </c>
       <c r="M7" s="4">
         <f t="shared" si="3"/>
-        <v>11002.75</v>
+        <v>916.89583333333337</v>
       </c>
       <c r="N7" s="4">
-        <f>MIN(0.055*P7,MAX(0.2*P7,972))</f>
-        <v>11002.75</v>
+        <f>MIN(0.055*P7,MAX(0.2*P7,972))/12</f>
+        <v>916.89583333333337</v>
       </c>
       <c r="P7">
         <f t="shared" si="1"/>

</xml_diff>